<commit_message>
Update easy aerobic run duration to 70 minutes and modify training plan spreadsheet formatting, by hand
</commit_message>
<xml_diff>
--- a/training_plan.xlsx
+++ b/training_plan.xlsx
@@ -921,7 +921,7 @@
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26">
@@ -950,7 +950,7 @@
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="82">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="90">
@@ -2823,7 +2823,7 @@
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="106">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="107">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="110">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="112">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="118">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121">
@@ -3687,7 +3687,7 @@
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123">

</xml_diff>

<commit_message>
Update training plan spreadsheet with revised data
</commit_message>
<xml_diff>
--- a/training_plan.xlsx
+++ b/training_plan.xlsx
@@ -49,12 +49,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -609,7 +610,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -638,7 +639,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -657,17 +658,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>T20</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
@@ -691,12 +692,12 @@
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
@@ -725,7 +726,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="n">
         <v>1</v>
@@ -744,17 +745,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T20</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" t="n">
         <v>1</v>
@@ -778,12 +779,12 @@
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
@@ -807,12 +808,12 @@
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -831,7 +832,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>E4x10s</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -841,7 +842,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -870,7 +871,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="n">
         <v>1</v>
@@ -897,7 +898,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" t="n">
         <v>2</v>
@@ -921,12 +922,12 @@
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
@@ -950,12 +951,12 @@
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" t="n">
         <v>2</v>
@@ -984,7 +985,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -1008,12 +1009,12 @@
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" t="n">
         <v>2</v>
@@ -1037,12 +1038,12 @@
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B30" t="n">
         <v>2</v>
@@ -1071,7 +1072,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B31" t="n">
         <v>2</v>
@@ -1095,12 +1096,12 @@
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B32" t="n">
         <v>2</v>
@@ -1129,7 +1130,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B33" t="n">
         <v>2</v>
@@ -1158,7 +1159,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="n">
         <v>2</v>
@@ -1185,7 +1186,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B35" t="n">
         <v>3</v>
@@ -1209,12 +1210,12 @@
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B36" t="n">
         <v>3</v>
@@ -1238,12 +1239,12 @@
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B37" t="n">
         <v>3</v>
@@ -1272,7 +1273,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B38" t="n">
         <v>3</v>
@@ -1296,12 +1297,12 @@
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B39" t="n">
         <v>3</v>
@@ -1325,12 +1326,12 @@
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B40" t="n">
         <v>3</v>
@@ -1359,7 +1360,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B41" t="n">
         <v>3</v>
@@ -1383,12 +1384,12 @@
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B42" t="n">
         <v>3</v>
@@ -1417,7 +1418,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B43" t="n">
         <v>3</v>
@@ -1446,7 +1447,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B44" t="n">
         <v>3</v>
@@ -1473,7 +1474,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" t="n">
         <v>4</v>
@@ -1497,12 +1498,12 @@
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B46" t="n">
         <v>4</v>
@@ -1526,12 +1527,12 @@
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B47" t="n">
         <v>4</v>
@@ -1560,7 +1561,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B48" t="n">
         <v>4</v>
@@ -1584,12 +1585,12 @@
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B49" t="n">
         <v>4</v>
@@ -1613,12 +1614,12 @@
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B50" t="n">
         <v>4</v>
@@ -1647,7 +1648,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51" t="n">
         <v>4</v>
@@ -1671,12 +1672,12 @@
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B52" t="n">
         <v>4</v>
@@ -1705,7 +1706,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B53" t="n">
         <v>4</v>
@@ -1734,7 +1735,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B54" t="n">
         <v>4</v>
@@ -1761,7 +1762,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B55" t="n">
         <v>5</v>
@@ -1790,7 +1791,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B56" t="n">
         <v>5</v>
@@ -1809,17 +1810,17 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>T20</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B57" t="n">
         <v>5</v>
@@ -1843,12 +1844,12 @@
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B58" t="n">
         <v>5</v>
@@ -1877,7 +1878,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B59" t="n">
         <v>5</v>
@@ -1896,17 +1897,17 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T20</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B60" t="n">
         <v>5</v>
@@ -1930,12 +1931,12 @@
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B61" t="n">
         <v>5</v>
@@ -1959,12 +1960,12 @@
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B62" t="n">
         <v>5</v>
@@ -1983,17 +1984,17 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>E4x10s</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B63" t="n">
         <v>5</v>
@@ -2022,7 +2023,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B64" t="n">
         <v>5</v>
@@ -2049,7 +2050,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B65" t="n">
         <v>6</v>
@@ -2073,12 +2074,12 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B66" t="n">
         <v>6</v>
@@ -2102,12 +2103,12 @@
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B67" t="n">
         <v>6</v>
@@ -2136,7 +2137,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B68" t="n">
         <v>6</v>
@@ -2160,12 +2161,12 @@
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B69" t="n">
         <v>6</v>
@@ -2189,12 +2190,12 @@
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B70" t="n">
         <v>6</v>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B71" t="n">
         <v>6</v>
@@ -2247,12 +2248,12 @@
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B72" t="n">
         <v>6</v>
@@ -2281,7 +2282,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B73" t="n">
         <v>6</v>
@@ -2310,7 +2311,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B74" t="n">
         <v>6</v>
@@ -2337,7 +2338,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B75" t="n">
         <v>7</v>
@@ -2361,12 +2362,12 @@
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B76" t="n">
         <v>7</v>
@@ -2390,12 +2391,12 @@
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B77" t="n">
         <v>7</v>
@@ -2424,7 +2425,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B78" t="n">
         <v>7</v>
@@ -2448,12 +2449,12 @@
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B79" t="n">
         <v>7</v>
@@ -2477,12 +2478,12 @@
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B80" t="n">
         <v>7</v>
@@ -2511,7 +2512,7 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B81" t="n">
         <v>7</v>
@@ -2535,12 +2536,12 @@
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B82" t="n">
         <v>7</v>
@@ -2569,7 +2570,7 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B83" t="n">
         <v>7</v>
@@ -2598,7 +2599,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B84" t="n">
         <v>7</v>
@@ -2625,7 +2626,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B85" t="n">
         <v>8</v>
@@ -2649,12 +2650,12 @@
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B86" t="n">
         <v>8</v>
@@ -2678,12 +2679,12 @@
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B87" t="n">
         <v>8</v>
@@ -2712,7 +2713,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B88" t="n">
         <v>8</v>
@@ -2736,12 +2737,12 @@
       </c>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B89" t="n">
         <v>8</v>
@@ -2765,12 +2766,12 @@
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B90" t="n">
         <v>8</v>
@@ -2799,7 +2800,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B91" t="n">
         <v>8</v>
@@ -2823,12 +2824,12 @@
       </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B92" t="n">
         <v>8</v>
@@ -2857,7 +2858,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B93" t="n">
         <v>8</v>
@@ -2886,7 +2887,7 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B94" t="n">
         <v>8</v>
@@ -2913,7 +2914,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B95" t="n">
         <v>9</v>
@@ -2942,7 +2943,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B96" t="n">
         <v>9</v>
@@ -2961,17 +2962,17 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>T20</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B97" t="n">
         <v>9</v>
@@ -3000,7 +3001,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B98" t="n">
         <v>9</v>
@@ -3029,7 +3030,7 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B99" t="n">
         <v>9</v>
@@ -3048,17 +3049,17 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T20</t>
         </is>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B100" t="n">
         <v>9</v>
@@ -3087,7 +3088,7 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B101" t="n">
         <v>9</v>
@@ -3116,7 +3117,7 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B102" t="n">
         <v>9</v>
@@ -3135,17 +3136,17 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>E4x10s</t>
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B103" t="n">
         <v>9</v>
@@ -3174,7 +3175,7 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B104" t="n">
         <v>9</v>
@@ -3201,7 +3202,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B105" t="n">
         <v>10</v>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B106" t="n">
         <v>10</v>
@@ -3259,7 +3260,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B107" t="n">
         <v>10</v>
@@ -3288,7 +3289,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B108" t="n">
         <v>10</v>
@@ -3317,7 +3318,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B109" t="n">
         <v>10</v>
@@ -3346,7 +3347,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B110" t="n">
         <v>10</v>
@@ -3375,7 +3376,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B111" t="n">
         <v>10</v>
@@ -3404,7 +3405,7 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B112" t="n">
         <v>10</v>
@@ -3433,7 +3434,7 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B113" t="n">
         <v>10</v>
@@ -3462,7 +3463,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B114" t="n">
         <v>10</v>
@@ -3489,7 +3490,7 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B115" t="n">
         <v>11</v>
@@ -3518,7 +3519,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B116" t="n">
         <v>11</v>
@@ -3537,17 +3538,17 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>T20</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B117" t="n">
         <v>11</v>
@@ -3576,7 +3577,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B118" t="n">
         <v>11</v>
@@ -3605,7 +3606,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B119" t="n">
         <v>11</v>
@@ -3624,17 +3625,17 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T20</t>
         </is>
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B120" t="n">
         <v>11</v>
@@ -3663,7 +3664,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B121" t="n">
         <v>11</v>
@@ -3692,7 +3693,7 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B122" t="n">
         <v>11</v>
@@ -3711,17 +3712,17 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>E4x10s</t>
         </is>
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B123" t="n">
         <v>11</v>
@@ -3750,7 +3751,7 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B124" t="n">
         <v>11</v>
@@ -3777,7 +3778,7 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B125" t="n">
         <v>12</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B126" t="n">
         <v>12</v>
@@ -3870,15 +3871,15 @@
       <c r="A130" t="n">
         <v>1</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="3">
         <f>SUM(G15:G24)</f>
         <v/>
       </c>
-      <c r="C130">
+      <c r="C130" s="3">
         <f>SUM(H15:H24)/60</f>
         <v/>
       </c>
-      <c r="D130">
+      <c r="D130" s="3">
         <f>B130 + (C130*60)/$B$13</f>
         <v/>
       </c>
@@ -3887,15 +3888,15 @@
       <c r="A131" t="n">
         <v>2</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="3">
         <f>SUM(G25:G34)</f>
         <v/>
       </c>
-      <c r="C131">
+      <c r="C131" s="3">
         <f>SUM(H25:H34)/60</f>
         <v/>
       </c>
-      <c r="D131">
+      <c r="D131" s="3">
         <f>B131 + (C131*60)/$B$13</f>
         <v/>
       </c>
@@ -3904,15 +3905,15 @@
       <c r="A132" t="n">
         <v>3</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="3">
         <f>SUM(G35:G44)</f>
         <v/>
       </c>
-      <c r="C132">
+      <c r="C132" s="3">
         <f>SUM(H35:H44)/60</f>
         <v/>
       </c>
-      <c r="D132">
+      <c r="D132" s="3">
         <f>B132 + (C132*60)/$B$13</f>
         <v/>
       </c>
@@ -3921,15 +3922,15 @@
       <c r="A133" t="n">
         <v>4</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="3">
         <f>SUM(G45:G54)</f>
         <v/>
       </c>
-      <c r="C133">
+      <c r="C133" s="3">
         <f>SUM(H45:H54)/60</f>
         <v/>
       </c>
-      <c r="D133">
+      <c r="D133" s="3">
         <f>B133 + (C133*60)/$B$13</f>
         <v/>
       </c>
@@ -3938,15 +3939,15 @@
       <c r="A134" t="n">
         <v>5</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="3">
         <f>SUM(G55:G64)</f>
         <v/>
       </c>
-      <c r="C134">
+      <c r="C134" s="3">
         <f>SUM(H55:H64)/60</f>
         <v/>
       </c>
-      <c r="D134">
+      <c r="D134" s="3">
         <f>B134 + (C134*60)/$B$13</f>
         <v/>
       </c>
@@ -3955,15 +3956,15 @@
       <c r="A135" t="n">
         <v>6</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="3">
         <f>SUM(G65:G74)</f>
         <v/>
       </c>
-      <c r="C135">
+      <c r="C135" s="3">
         <f>SUM(H65:H74)/60</f>
         <v/>
       </c>
-      <c r="D135">
+      <c r="D135" s="3">
         <f>B135 + (C135*60)/$B$13</f>
         <v/>
       </c>
@@ -3972,15 +3973,15 @@
       <c r="A136" t="n">
         <v>7</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="3">
         <f>SUM(G75:G84)</f>
         <v/>
       </c>
-      <c r="C136">
+      <c r="C136" s="3">
         <f>SUM(H75:H84)/60</f>
         <v/>
       </c>
-      <c r="D136">
+      <c r="D136" s="3">
         <f>B136 + (C136*60)/$B$13</f>
         <v/>
       </c>
@@ -3989,15 +3990,15 @@
       <c r="A137" t="n">
         <v>8</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="3">
         <f>SUM(G85:G94)</f>
         <v/>
       </c>
-      <c r="C137">
+      <c r="C137" s="3">
         <f>SUM(H85:H94)/60</f>
         <v/>
       </c>
-      <c r="D137">
+      <c r="D137" s="3">
         <f>B137 + (C137*60)/$B$13</f>
         <v/>
       </c>
@@ -4006,15 +4007,15 @@
       <c r="A138" t="n">
         <v>9</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="3">
         <f>SUM(G95:G104)</f>
         <v/>
       </c>
-      <c r="C138">
+      <c r="C138" s="3">
         <f>SUM(H95:H104)/60</f>
         <v/>
       </c>
-      <c r="D138">
+      <c r="D138" s="3">
         <f>B138 + (C138*60)/$B$13</f>
         <v/>
       </c>
@@ -4023,15 +4024,15 @@
       <c r="A139" t="n">
         <v>10</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="3">
         <f>SUM(G105:G114)</f>
         <v/>
       </c>
-      <c r="C139">
+      <c r="C139" s="3">
         <f>SUM(H105:H114)/60</f>
         <v/>
       </c>
-      <c r="D139">
+      <c r="D139" s="3">
         <f>B139 + (C139*60)/$B$13</f>
         <v/>
       </c>
@@ -4040,15 +4041,15 @@
       <c r="A140" t="n">
         <v>11</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="3">
         <f>SUM(G115:G124)</f>
         <v/>
       </c>
-      <c r="C140">
+      <c r="C140" s="3">
         <f>SUM(H115:H124)/60</f>
         <v/>
       </c>
-      <c r="D140">
+      <c r="D140" s="3">
         <f>B140 + (C140*60)/$B$13</f>
         <v/>
       </c>
@@ -4057,15 +4058,15 @@
       <c r="A141" t="n">
         <v>12</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="3">
         <f>SUM(G125:G126)</f>
         <v/>
       </c>
-      <c r="C141">
+      <c r="C141" s="3">
         <f>SUM(H125:H126)/60</f>
         <v/>
       </c>
-      <c r="D141">
+      <c r="D141" s="3">
         <f>B141 + (C141*60)/$B$13</f>
         <v/>
       </c>
@@ -4107,15 +4108,15 @@
       <c r="A145" t="n">
         <v>1</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="3">
         <f>SUM(G15:G21)</f>
         <v/>
       </c>
-      <c r="C145">
+      <c r="C145" s="3">
         <f>SUM(H15:H21)/60</f>
         <v/>
       </c>
-      <c r="D145">
+      <c r="D145" s="3">
         <f>B145 + (C145*60)/$B$13</f>
         <v/>
       </c>
@@ -4124,15 +4125,15 @@
       <c r="A146" t="n">
         <v>2</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="3">
         <f>SUM(G22:G28)</f>
         <v/>
       </c>
-      <c r="C146">
+      <c r="C146" s="3">
         <f>SUM(H22:H28)/60</f>
         <v/>
       </c>
-      <c r="D146">
+      <c r="D146" s="3">
         <f>B146 + (C146*60)/$B$13</f>
         <v/>
       </c>
@@ -4141,15 +4142,15 @@
       <c r="A147" t="n">
         <v>3</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="3">
         <f>SUM(G29:G35)</f>
         <v/>
       </c>
-      <c r="C147">
+      <c r="C147" s="3">
         <f>SUM(H29:H35)/60</f>
         <v/>
       </c>
-      <c r="D147">
+      <c r="D147" s="3">
         <f>B147 + (C147*60)/$B$13</f>
         <v/>
       </c>
@@ -4158,15 +4159,15 @@
       <c r="A148" t="n">
         <v>4</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="3">
         <f>SUM(G36:G42)</f>
         <v/>
       </c>
-      <c r="C148">
+      <c r="C148" s="3">
         <f>SUM(H36:H42)/60</f>
         <v/>
       </c>
-      <c r="D148">
+      <c r="D148" s="3">
         <f>B148 + (C148*60)/$B$13</f>
         <v/>
       </c>
@@ -4175,15 +4176,15 @@
       <c r="A149" t="n">
         <v>5</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="3">
         <f>SUM(G43:G49)</f>
         <v/>
       </c>
-      <c r="C149">
+      <c r="C149" s="3">
         <f>SUM(H43:H49)/60</f>
         <v/>
       </c>
-      <c r="D149">
+      <c r="D149" s="3">
         <f>B149 + (C149*60)/$B$13</f>
         <v/>
       </c>
@@ -4192,15 +4193,15 @@
       <c r="A150" t="n">
         <v>6</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="3">
         <f>SUM(G50:G56)</f>
         <v/>
       </c>
-      <c r="C150">
+      <c r="C150" s="3">
         <f>SUM(H50:H56)/60</f>
         <v/>
       </c>
-      <c r="D150">
+      <c r="D150" s="3">
         <f>B150 + (C150*60)/$B$13</f>
         <v/>
       </c>
@@ -4209,15 +4210,15 @@
       <c r="A151" t="n">
         <v>7</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="3">
         <f>SUM(G57:G63)</f>
         <v/>
       </c>
-      <c r="C151">
+      <c r="C151" s="3">
         <f>SUM(H57:H63)/60</f>
         <v/>
       </c>
-      <c r="D151">
+      <c r="D151" s="3">
         <f>B151 + (C151*60)/$B$13</f>
         <v/>
       </c>
@@ -4226,15 +4227,15 @@
       <c r="A152" t="n">
         <v>8</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="3">
         <f>SUM(G64:G70)</f>
         <v/>
       </c>
-      <c r="C152">
+      <c r="C152" s="3">
         <f>SUM(H64:H70)/60</f>
         <v/>
       </c>
-      <c r="D152">
+      <c r="D152" s="3">
         <f>B152 + (C152*60)/$B$13</f>
         <v/>
       </c>
@@ -4243,15 +4244,15 @@
       <c r="A153" t="n">
         <v>9</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="3">
         <f>SUM(G71:G77)</f>
         <v/>
       </c>
-      <c r="C153">
+      <c r="C153" s="3">
         <f>SUM(H71:H77)/60</f>
         <v/>
       </c>
-      <c r="D153">
+      <c r="D153" s="3">
         <f>B153 + (C153*60)/$B$13</f>
         <v/>
       </c>
@@ -4260,15 +4261,15 @@
       <c r="A154" t="n">
         <v>10</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="3">
         <f>SUM(G78:G84)</f>
         <v/>
       </c>
-      <c r="C154">
+      <c r="C154" s="3">
         <f>SUM(H78:H84)/60</f>
         <v/>
       </c>
-      <c r="D154">
+      <c r="D154" s="3">
         <f>B154 + (C154*60)/$B$13</f>
         <v/>
       </c>
@@ -4277,15 +4278,15 @@
       <c r="A155" t="n">
         <v>11</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="3">
         <f>SUM(G85:G91)</f>
         <v/>
       </c>
-      <c r="C155">
+      <c r="C155" s="3">
         <f>SUM(H85:H91)/60</f>
         <v/>
       </c>
-      <c r="D155">
+      <c r="D155" s="3">
         <f>B155 + (C155*60)/$B$13</f>
         <v/>
       </c>
@@ -4294,15 +4295,15 @@
       <c r="A156" t="n">
         <v>12</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="3">
         <f>SUM(G92:G98)</f>
         <v/>
       </c>
-      <c r="C156">
+      <c r="C156" s="3">
         <f>SUM(H92:H98)/60</f>
         <v/>
       </c>
-      <c r="D156">
+      <c r="D156" s="3">
         <f>B156 + (C156*60)/$B$13</f>
         <v/>
       </c>
@@ -4311,15 +4312,15 @@
       <c r="A157" t="n">
         <v>13</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="3">
         <f>SUM(G99:G105)</f>
         <v/>
       </c>
-      <c r="C157">
+      <c r="C157" s="3">
         <f>SUM(H99:H105)/60</f>
         <v/>
       </c>
-      <c r="D157">
+      <c r="D157" s="3">
         <f>B157 + (C157*60)/$B$13</f>
         <v/>
       </c>
@@ -4328,15 +4329,15 @@
       <c r="A158" t="n">
         <v>14</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="3">
         <f>SUM(G106:G112)</f>
         <v/>
       </c>
-      <c r="C158">
+      <c r="C158" s="3">
         <f>SUM(H106:H112)/60</f>
         <v/>
       </c>
-      <c r="D158">
+      <c r="D158" s="3">
         <f>B158 + (C158*60)/$B$13</f>
         <v/>
       </c>
@@ -4345,15 +4346,15 @@
       <c r="A159" t="n">
         <v>15</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="3">
         <f>SUM(G113:G119)</f>
         <v/>
       </c>
-      <c r="C159">
+      <c r="C159" s="3">
         <f>SUM(H113:H119)/60</f>
         <v/>
       </c>
-      <c r="D159">
+      <c r="D159" s="3">
         <f>B159 + (C159*60)/$B$13</f>
         <v/>
       </c>
@@ -4362,15 +4363,15 @@
       <c r="A160" t="n">
         <v>16</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="3">
         <f>SUM(G120:G126)</f>
         <v/>
       </c>
-      <c r="C160">
+      <c r="C160" s="3">
         <f>SUM(H120:H126)/60</f>
         <v/>
       </c>
-      <c r="D160">
+      <c r="D160" s="3">
         <f>B160 + (C160*60)/$B$13</f>
         <v/>
       </c>

</xml_diff>